<commit_message>
Fixing some errors, gotta check what's up with the DU api key
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\ProductionStatement_DUProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F3546F-4663-42C9-932B-E05816B4D660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EC79C0-8049-4B95-839F-462C21688B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="282">
   <si>
     <t>Name</t>
   </si>
@@ -873,13 +873,22 @@
   </si>
   <si>
     <t>DispatcherQueuePath</t>
+  </si>
+  <si>
+    <t>Shared/ConocoProject</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetName</t>
+  </si>
+  <si>
+    <t>ConocoProject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -922,6 +931,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -944,7 +960,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -955,6 +971,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1273,7 +1290,7 @@
   <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1623,9 +1640,25 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6"/>
+    </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>